<commit_message>
Sept planting date and reproduction/yield needs to be improved, but the rest is improving Simplified phenology
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/GattonKylie.xlsx
+++ b/Prototypes/Mungbean/GattonKylie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9FA18C-6114-4F01-8841-633838BBECD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1B2E51-1D01-4916-B870-72C480941119}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2820" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kylie" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="18">
   <si>
     <t>site</t>
   </si>
@@ -933,7 +933,7 @@
   <dimension ref="A1:R4392"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1425" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C208" sqref="C208"/>
+      <selection activeCell="D1455" sqref="D1455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33897,7 +33897,7 @@
       <c r="D1438">
         <v>11.2</v>
       </c>
-      <c r="E1438">
+      <c r="E1438" s="1">
         <v>27.3</v>
       </c>
       <c r="F1438" s="1">
@@ -33920,7 +33920,7 @@
       <c r="D1439">
         <v>8.5</v>
       </c>
-      <c r="E1439">
+      <c r="E1439" s="1">
         <v>23.2</v>
       </c>
       <c r="F1439" s="1">
@@ -33943,7 +33943,7 @@
       <c r="D1440">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E1440">
+      <c r="E1440" s="1">
         <v>25.7</v>
       </c>
       <c r="F1440" s="1">
@@ -33966,7 +33966,7 @@
       <c r="D1441">
         <v>20.6</v>
       </c>
-      <c r="E1441">
+      <c r="E1441" s="1">
         <v>30.8</v>
       </c>
       <c r="F1441" s="1">
@@ -33989,7 +33989,7 @@
       <c r="D1442">
         <v>27.3</v>
       </c>
-      <c r="E1442">
+      <c r="E1442" s="1">
         <v>31.9</v>
       </c>
       <c r="F1442" s="1">
@@ -34012,7 +34012,7 @@
       <c r="D1443">
         <v>16.399999999999999</v>
       </c>
-      <c r="E1443">
+      <c r="E1443" s="1">
         <v>32.299999999999997</v>
       </c>
       <c r="F1443" s="1">
@@ -34035,7 +34035,7 @@
       <c r="D1444">
         <v>26.5</v>
       </c>
-      <c r="E1444">
+      <c r="E1444" s="1">
         <v>28.4</v>
       </c>
       <c r="F1444" s="1">
@@ -34058,7 +34058,7 @@
       <c r="D1445">
         <v>22.1</v>
       </c>
-      <c r="E1445">
+      <c r="E1445" s="1">
         <v>28.8</v>
       </c>
       <c r="F1445" s="1">
@@ -34081,7 +34081,7 @@
       <c r="D1446">
         <v>17.399999999999999</v>
       </c>
-      <c r="E1446">
+      <c r="E1446" s="1">
         <v>30.4</v>
       </c>
       <c r="F1446" s="1">
@@ -34104,7 +34104,7 @@
       <c r="D1447">
         <v>11.6</v>
       </c>
-      <c r="E1447">
+      <c r="E1447" s="1">
         <v>28.7</v>
       </c>
       <c r="F1447" s="1">
@@ -34127,7 +34127,7 @@
       <c r="D1448">
         <v>25.4</v>
       </c>
-      <c r="E1448">
+      <c r="E1448" s="1">
         <v>31.8</v>
       </c>
       <c r="F1448" s="1">
@@ -34150,7 +34150,7 @@
       <c r="D1449">
         <v>25.5</v>
       </c>
-      <c r="E1449">
+      <c r="E1449" s="1">
         <v>29.9</v>
       </c>
       <c r="F1449" s="1">
@@ -34173,7 +34173,7 @@
       <c r="D1450">
         <v>29.4</v>
       </c>
-      <c r="E1450">
+      <c r="E1450" s="1">
         <v>30.1</v>
       </c>
       <c r="F1450" s="1">
@@ -34196,7 +34196,7 @@
       <c r="D1451">
         <v>21</v>
       </c>
-      <c r="E1451">
+      <c r="E1451" s="1">
         <v>29.8</v>
       </c>
       <c r="F1451" s="1">
@@ -34219,7 +34219,7 @@
       <c r="D1452">
         <v>29.7</v>
       </c>
-      <c r="E1452">
+      <c r="E1452" s="1">
         <v>29.9</v>
       </c>
       <c r="F1452" s="1">
@@ -34242,7 +34242,7 @@
       <c r="D1453">
         <v>30.7</v>
       </c>
-      <c r="E1453">
+      <c r="E1453" s="1">
         <v>30.6</v>
       </c>
       <c r="F1453" s="1">
@@ -34265,7 +34265,7 @@
       <c r="D1454">
         <v>30</v>
       </c>
-      <c r="E1454">
+      <c r="E1454" s="1">
         <v>30.8</v>
       </c>
       <c r="F1454" s="1">
@@ -34288,7 +34288,7 @@
       <c r="D1455">
         <v>23.8</v>
       </c>
-      <c r="E1455">
+      <c r="E1455" s="1">
         <v>32.700000000000003</v>
       </c>
       <c r="F1455" s="1">
@@ -34311,7 +34311,7 @@
       <c r="D1456">
         <v>20</v>
       </c>
-      <c r="E1456">
+      <c r="E1456" s="1">
         <v>31.4</v>
       </c>
       <c r="F1456" s="1">
@@ -34332,9 +34332,9 @@
         <v>352</v>
       </c>
       <c r="D1457">
-        <v>26.1</v>
-      </c>
-      <c r="E1457">
+        <v>25</v>
+      </c>
+      <c r="E1457" s="1">
         <v>31.2</v>
       </c>
       <c r="F1457" s="1">
@@ -34357,7 +34357,7 @@
       <c r="D1458">
         <v>26.8</v>
       </c>
-      <c r="E1458">
+      <c r="E1458" s="1">
         <v>32</v>
       </c>
       <c r="F1458" s="1">
@@ -34378,10 +34378,10 @@
         <v>354</v>
       </c>
       <c r="D1459">
-        <v>24.7</v>
-      </c>
-      <c r="E1459">
-        <v>31.4</v>
+        <v>24.5</v>
+      </c>
+      <c r="E1459" s="1">
+        <v>34.4</v>
       </c>
       <c r="F1459" s="1">
         <v>17.3</v>
@@ -34391,19 +34391,73 @@
       </c>
     </row>
     <row r="1460" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1460" s="4"/>
-      <c r="F1460" s="1"/>
-      <c r="G1460" s="1"/>
+      <c r="A1460" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1460" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C1460">
+        <v>355</v>
+      </c>
+      <c r="D1460">
+        <v>24.1</v>
+      </c>
+      <c r="E1460" s="1">
+        <v>34</v>
+      </c>
+      <c r="F1460" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="G1460" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="1461" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1461" s="4"/>
-      <c r="F1461" s="1"/>
-      <c r="G1461" s="1"/>
+      <c r="A1461" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1461" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C1461">
+        <v>356</v>
+      </c>
+      <c r="D1461">
+        <v>23.9</v>
+      </c>
+      <c r="E1461" s="1">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="F1461" s="1">
+        <v>18.7</v>
+      </c>
+      <c r="G1461" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="1462" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1462" s="4"/>
-      <c r="F1462" s="1"/>
-      <c r="G1462" s="1"/>
+      <c r="A1462" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1462" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C1462">
+        <v>357</v>
+      </c>
+      <c r="D1462">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E1462" s="1">
+        <v>31.4</v>
+      </c>
+      <c r="F1462" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="G1462" s="1">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="1463" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1463" s="4"/>

</xml_diff>